<commit_message>
Updated Topical Areas for 3.10
There is variation on the use of series as a folder or category leader.
These were some of the ones I recall having trouble with: Artober,
Hispanic Heritage, Virtuoso. I have updated these and will test out
Virtuoso in a spreadsheet this week.
</commit_message>
<xml_diff>
--- a/20140722_TOPICAL_AREAS_SHEET_REVISION.xlsx
+++ b/20140722_TOPICAL_AREAS_SHEET_REVISION.xlsx
@@ -14,10 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="200">
-  <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Hispanic Heritage Month:/user/agrp_calsuite-MainCampus/Series/Hispanic Heritage Month</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="210">
   <si>
     <t>2a3e9efe-40ed9887-0140-ee844b42-000004aa</t>
   </si>
@@ -25,15 +22,6 @@
     <t>series/Hispanic Heritage Month</t>
   </si>
   <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Community:/user/agrp_calsuite-MainCampus/series/Community</t>
-  </si>
-  <si>
-    <t>2a3e9efe-4135b172-0141-3803bdaa-0000194d</t>
-  </si>
-  <si>
-    <t>series/Community</t>
-  </si>
-  <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Outreach:/user/agrp_calsuite-MainCampus/Outreach</t>
   </si>
   <si>
@@ -43,15 +31,9 @@
     <t>Outreach</t>
   </si>
   <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Artober:/user/agrp_calsuite-MainCampus/Artober</t>
-  </si>
-  <si>
     <t>2a3e9efe-3948a864-0139-58c00d23-00006346</t>
   </si>
   <si>
-    <t>Artober</t>
-  </si>
-  <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Writing:/user/agrp_calsuite-MainCampus/Writing</t>
   </si>
   <si>
@@ -61,15 +43,6 @@
     <t>Writing</t>
   </si>
   <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Theater:/user/agrp_calsuite-MainCampus/Theater</t>
-  </si>
-  <si>
-    <t>ff808181-1fd73b03-011f-d73b065c-00000002</t>
-  </si>
-  <si>
-    <t>Theater</t>
-  </si>
-  <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Teens:/user/agrp_calsuite-MainCampus/Teens</t>
   </si>
   <si>
@@ -124,36 +97,21 @@
     <t>series/Writers Circle</t>
   </si>
   <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Wishing Chair Productions:/user/agrp_calsuite-MainCampus/Series/Wishing Chair Productions</t>
-  </si>
-  <si>
     <t>2a3e9efe-334bc29f-0133-7a00e56f-000036cc</t>
   </si>
   <si>
     <t>series/Wishing Chair Productions</t>
   </si>
   <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Thinking Out of the Lunch Box:/user/agrp_calsuite-MainCampus/Series/Thinking Out of the Lunch Box</t>
-  </si>
-  <si>
     <t>2a3e9efe-39249ad8-0139-45fd718a-0000434b</t>
   </si>
   <si>
     <t>series/Thinking Out of the Lunch Box</t>
   </si>
   <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Summer Reading:/user/agrp_calsuite-MainCampus/series/Summer Reading</t>
-  </si>
-  <si>
     <t>2a3e9efe-3c9a9aa5-013c-a733b8e3-00007021</t>
   </si>
   <si>
-    <t>series/Summer Reading</t>
-  </si>
-  <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Salon@615:/user/agrp_calsuite-MainCampus/series/Salon@615</t>
-  </si>
-  <si>
     <t>2a3e9efe-334bc29f-0133-7a04041e-000036d1</t>
   </si>
   <si>
@@ -187,9 +145,6 @@
     <t>series/NCAA</t>
   </si>
   <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Movies @ Main:/user/agrp_calsuite-MainCampus/series/Movies @ Main</t>
-  </si>
-  <si>
     <t>2a3e9efe-334bc29f-0133-7a02c06c-000036cf</t>
   </si>
   <si>
@@ -214,15 +169,9 @@
     <t>series/Holiday</t>
   </si>
   <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Concerts in the Courtyard:/user/agrp_calsuite-MainCampus/series/Concerts in the Courtyard</t>
-  </si>
-  <si>
     <t>2a3e9efe-334bc29f-0133-7a0374b5-000036d0</t>
   </si>
   <si>
-    <t>series/Concerts in the Courtyard</t>
-  </si>
-  <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Community of Many Faces:/user/agrp_calsuite-MainCampus/series/Community of Many Faces</t>
   </si>
   <si>
@@ -250,45 +199,21 @@
     <t>series/Closed</t>
   </si>
   <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Classical Guitar:/user/agrp_calsuite-MainCampus/series/Classical Guitar</t>
-  </si>
-  <si>
     <t>2a3e9efe-3948a864-0139-58cae8e7-000063e9</t>
   </si>
   <si>
-    <t>series/Classical Guitar</t>
-  </si>
-  <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Artober:/user/agrp_calsuite-MainCampus/Series/Artober</t>
-  </si>
-  <si>
     <t>series/Artober</t>
   </si>
   <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Sale:/user/agrp_calsuite-MainCampus/Sale</t>
-  </si>
-  <si>
     <t>2a3e9efe-34870943-0134-8a28d156-00000286</t>
   </si>
   <si>
-    <t>Sale</t>
-  </si>
-  <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Personal Finance:/user/agrp_calsuite-MainCampus/Personal Finance</t>
-  </si>
-  <si>
     <t>2a3e9efe-334bc29f-0133-f14fd5fa-00001df8</t>
   </si>
   <si>
-    <t>Personal Finance</t>
-  </si>
-  <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Music:/user/agrp_calsuite-MainCampus/Music</t>
   </si>
   <si>
-    <t>402881e6-20a21413-0120-a24bc8db-00000056</t>
-  </si>
-  <si>
     <t>Music</t>
   </si>
   <si>
@@ -364,24 +289,9 @@
     <t>location/North</t>
   </si>
   <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Metro Archives:/user/agrp_calsuite-MainCampus/Metro Archives</t>
-  </si>
-  <si>
-    <t>2a3e9efe-334bc29f-0133-79befbc0-00003692</t>
-  </si>
-  <si>
-    <t>location/Metro Archives</t>
-  </si>
-  <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=MAIN (Downtown):/user/agrp_calsuite-MainCampus/Locations/MAIN</t>
-  </si>
-  <si>
     <t>ff808181-1fd7389e-011f-d7389fa2-00000028</t>
   </si>
   <si>
-    <t>location/Main (Downtown)</t>
-  </si>
-  <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Madison:/user/agrp_calsuite-MainCampus/Madison</t>
   </si>
   <si>
@@ -517,24 +427,12 @@
     <t>Home and Garden</t>
   </si>
   <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Health:/user/agrp_calsuite-MainCampus/Health</t>
-  </si>
-  <si>
     <t>2a3e9efe-35dd67b8-0135-e8eb41e5-000012f4</t>
   </si>
   <si>
-    <t>Health</t>
-  </si>
-  <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Featured:/user/agrp_calsuite-MainCampus/Featured</t>
-  </si>
-  <si>
     <t>2a3e9efe-35dd67b8-0135-f8474b67-00005c80</t>
   </si>
   <si>
-    <t>Featured</t>
-  </si>
-  <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Exhibits:/user/agrp_calsuite-MainCampus/Exhibits</t>
   </si>
   <si>
@@ -544,24 +442,12 @@
     <t>Exhibits</t>
   </si>
   <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Dance:/user/agrp_calsuite-MainCampus/Dance</t>
-  </si>
-  <si>
     <t>ff808181-1fd7389e-011f-d7389ef9-00000003</t>
   </si>
   <si>
-    <t>Dance</t>
-  </si>
-  <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Computers:/user/agrp_calsuite-MainCampus/Computers</t>
-  </si>
-  <si>
     <t>2a3e9efe-334bc29f-0133-f14ece3f-00001df3</t>
   </si>
   <si>
-    <t>Computers</t>
-  </si>
-  <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Children:/user/agrp_calsuite-MainCampus/Children</t>
   </si>
   <si>
@@ -571,15 +457,6 @@
     <t>Children</t>
   </si>
   <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Business:/user/agrp_calsuite-MainCampus/Business</t>
-  </si>
-  <si>
-    <t>2a3e9efe-334bc29f-0133-f14fa578-00001df6</t>
-  </si>
-  <si>
-    <t>Business</t>
-  </si>
-  <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Book Clubs:/user/agrp_calsuite-MainCampus/Book Clubs</t>
   </si>
   <si>
@@ -589,21 +466,9 @@
     <t>Book Clubs</t>
   </si>
   <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Authors:/user/agrp_calsuite-MainCampus/Authors</t>
-  </si>
-  <si>
     <t>ff808181-1fd73b03-011f-d73b06f8-0000000c</t>
   </si>
   <si>
-    <t>Authors</t>
-  </si>
-  <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Arts &amp; Crafts:/user/agrp_calsuite-MainCampus/Arts &amp; Crafts</t>
-  </si>
-  <si>
-    <t>ff808181-1fd7389e-011f-d7389ecc-00000001</t>
-  </si>
-  <si>
     <t>Arts and Crafts</t>
   </si>
   <si>
@@ -614,6 +479,171 @@
   </si>
   <si>
     <t>TOPICAL AREA LABEL</t>
+  </si>
+  <si>
+    <t>Author Talks</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Author Talks:/user/agrp_calsuite-MainCampus/Author Talks</t>
+  </si>
+  <si>
+    <t>2a3e9ebb-47c63158-0147-c6315859-00000000</t>
+  </si>
+  <si>
+    <t>Computers and Technology</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Computers and Technology:/user/agrp_calsuite-MainCampus/Computers and Technology</t>
+  </si>
+  <si>
+    <t>Dance and Theater</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Dance and Theater:/user/agrp_calsuite-MainCampus/Dance and Theater</t>
+  </si>
+  <si>
+    <t>Health and Wellness</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Health and Wellnes:/user/agrp_calsuite-MainCampus/Health and Wellness</t>
+  </si>
+  <si>
+    <t>Homework Help</t>
+  </si>
+  <si>
+    <t>2a3e9efe-334bc29f-0133-f150031d-00001df9</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Homework Help:/user/agrp_calsuite-MainCampus/Homework Help</t>
+  </si>
+  <si>
+    <t>ff808181-1fd73b03-011f-d73b0642-00000001</t>
+  </si>
+  <si>
+    <t>Money and Taxes</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Money and Taxes:/user/agrp_calsuite-MainCampus/Money and Taxes</t>
+  </si>
+  <si>
+    <t>Book Sales</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Book Sales:/user/agrp_calsuite-MainCampus/Book Sales</t>
+  </si>
+  <si>
+    <t>series/African American History Month</t>
+  </si>
+  <si>
+    <t>2a3e9efe-432e9841-0143-3040dc3a-00000dcb</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/African American History Month:/user/agrp_calsuite-MainCampus/series/African American History Month</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Movies @ Main:/user/agrp_calsuite-MainCampus/series/Movies @ Main</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Salon@615:/user/agrp_calsuite-MainCampus/series/Salon@615</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Thinking Out of the Lunch Box:/user/agrp_calsuite-MainCampus/series/Thinking Out of the Lunch Box</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Artober:/user/agrp_calsuite-MainCampus/series/Artober</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Wishing Chair Productions:/user/agrp_calsuite-MainCampus/series/Wishing Chair Productions</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Hispanic Heritage Month:/user/agrp_calsuite-MainCampus/series/Hispanic Heritage Month</t>
+  </si>
+  <si>
+    <t>ff808181-1fd7389e-011f-d7389ed0-00000002</t>
+  </si>
+  <si>
+    <t>Puppet Shows</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Puppet Shows/user/agrp_calsuite-MainCampus/Puppet Shows</t>
+  </si>
+  <si>
+    <t>series/Hunger Awareness</t>
+  </si>
+  <si>
+    <t>2a3e9efe-432e9841-0143-303b3a57-00000dad</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Hunger Awareness:/user/agrp_calsuite-MainCampus/series/Hunger Awareness</t>
+  </si>
+  <si>
+    <t>Summer Challenge</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Summer Challenge/user/agrp_calsuite-MainCampus/Summer Challenge</t>
+  </si>
+  <si>
+    <t>Studio NPL</t>
+  </si>
+  <si>
+    <t>2a3e9ebb-47ca823e-0147-ca9c67cd-0000001e</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Studio NPL:/user/agrp_calsuite-MainCampus/Studio NPL</t>
+  </si>
+  <si>
+    <t>That Nashville Sound</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=That Nashville Sound:/user/agrp_calsuite-MainCampus/That Nashville Sound</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Arts and Crafts:/user/agrp_calsuite-MainCampus/Arts and Crafts</t>
+  </si>
+  <si>
+    <t>ESL</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=ESL:/user/agrp_calsuite-MainCampus/ESL</t>
+  </si>
+  <si>
+    <t>Courtyard Concerts</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Courtyard Concerts:/user/agrp_calsuite-MainCampus/series/Courtyard Concerts</t>
+  </si>
+  <si>
+    <t>First Tuesday at the Archives</t>
+  </si>
+  <si>
+    <t>2a3e9ebb-47ca823e-0147-ca9bba18-0000001c</t>
+  </si>
+  <si>
+    <t>2a3e9ebb-47ca823e-0147-ca9c9c61-0000001f</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=First Tuesday at the Archives:/user/agrp_calsuite-MainCampus/First Tuesday at the Archives</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=TOTAL:/user/agrp_calsuite-MainCampus/TOTAL</t>
+  </si>
+  <si>
+    <t>location/Main Library</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Main Library:/user/agrp_calsuite-MainCampus/Locations/Main Library</t>
+  </si>
+  <si>
+    <t>series/Virtuoso Showcase Classical Guitar</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Virtuoso Showcase Classical Guitar:/user/agrp_calsuite-MainCampus/series/Virtuoso Showcase Classical Guitar</t>
+  </si>
+  <si>
+    <t>2a3e9ebb-47ca823e-0147-ca9cd657-00000020</t>
   </si>
 </sst>
 </file>
@@ -970,9 +1000,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C78"/>
+  <dimension ref="A1:C70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -982,742 +1014,779 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>199</v>
+        <v>154</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>198</v>
+        <v>153</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>197</v>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>196</v>
+        <v>149</v>
       </c>
       <c r="B4" t="s">
-        <v>195</v>
+        <v>148</v>
       </c>
       <c r="C4" t="s">
-        <v>194</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>193</v>
+        <v>170</v>
       </c>
       <c r="B5" t="s">
-        <v>192</v>
+        <v>63</v>
       </c>
       <c r="C5" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>190</v>
+        <v>146</v>
       </c>
       <c r="B6" t="s">
-        <v>189</v>
+        <v>145</v>
       </c>
       <c r="C6" t="s">
-        <v>188</v>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>158</v>
+      </c>
+      <c r="B7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C7" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="B8" t="s">
-        <v>186</v>
+        <v>51</v>
       </c>
       <c r="C8" t="s">
-        <v>185</v>
+        <v>198</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>184</v>
+        <v>160</v>
       </c>
       <c r="B9" t="s">
-        <v>183</v>
+        <v>142</v>
       </c>
       <c r="C9" t="s">
-        <v>182</v>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>195</v>
+      </c>
+      <c r="B10" t="s">
+        <v>138</v>
+      </c>
+      <c r="C10" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>181</v>
+        <v>141</v>
       </c>
       <c r="B11" t="s">
-        <v>180</v>
+        <v>140</v>
       </c>
       <c r="C11" t="s">
-        <v>179</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>178</v>
+        <v>199</v>
       </c>
       <c r="B12" t="s">
-        <v>177</v>
+        <v>200</v>
       </c>
       <c r="C12" t="s">
-        <v>176</v>
+        <v>202</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="B13" t="s">
-        <v>174</v>
+        <v>137</v>
       </c>
       <c r="C13" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>172</v>
+        <v>136</v>
       </c>
       <c r="B14" t="s">
-        <v>171</v>
+        <v>135</v>
       </c>
       <c r="C14" t="s">
-        <v>170</v>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>164</v>
+      </c>
+      <c r="B15" t="s">
+        <v>165</v>
+      </c>
+      <c r="C15" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>169</v>
+        <v>133</v>
       </c>
       <c r="B16" t="s">
-        <v>168</v>
+        <v>132</v>
       </c>
       <c r="C16" t="s">
-        <v>167</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>166</v>
+        <v>130</v>
       </c>
       <c r="B17" t="s">
-        <v>165</v>
+        <v>129</v>
       </c>
       <c r="C17" t="s">
-        <v>164</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>163</v>
+        <v>127</v>
       </c>
       <c r="B18" t="s">
-        <v>162</v>
+        <v>126</v>
       </c>
       <c r="C18" t="s">
-        <v>161</v>
+        <v>125</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>160</v>
+        <v>124</v>
       </c>
       <c r="B19" t="s">
-        <v>159</v>
+        <v>123</v>
       </c>
       <c r="C19" t="s">
-        <v>158</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>157</v>
+        <v>121</v>
       </c>
       <c r="B20" t="s">
-        <v>156</v>
+        <v>120</v>
       </c>
       <c r="C20" t="s">
-        <v>155</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>154</v>
+        <v>118</v>
       </c>
       <c r="B21" t="s">
-        <v>153</v>
+        <v>117</v>
       </c>
       <c r="C21" t="s">
-        <v>152</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>151</v>
+        <v>115</v>
       </c>
       <c r="B22" t="s">
-        <v>150</v>
+        <v>114</v>
       </c>
       <c r="C22" t="s">
-        <v>149</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>148</v>
+        <v>112</v>
       </c>
       <c r="B23" t="s">
-        <v>147</v>
+        <v>111</v>
       </c>
       <c r="C23" t="s">
-        <v>146</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>145</v>
+        <v>109</v>
       </c>
       <c r="B24" t="s">
-        <v>144</v>
+        <v>108</v>
       </c>
       <c r="C24" t="s">
-        <v>143</v>
+        <v>107</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>142</v>
+        <v>106</v>
       </c>
       <c r="B25" t="s">
-        <v>141</v>
+        <v>105</v>
       </c>
       <c r="C25" t="s">
-        <v>140</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>139</v>
+        <v>103</v>
       </c>
       <c r="B26" t="s">
-        <v>138</v>
+        <v>102</v>
       </c>
       <c r="C26" t="s">
-        <v>137</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>136</v>
+        <v>100</v>
       </c>
       <c r="B27" t="s">
-        <v>135</v>
+        <v>99</v>
       </c>
       <c r="C27" t="s">
-        <v>134</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>133</v>
+        <v>97</v>
       </c>
       <c r="B28" t="s">
-        <v>132</v>
+        <v>96</v>
       </c>
       <c r="C28" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>130</v>
+        <v>94</v>
       </c>
       <c r="B29" t="s">
-        <v>129</v>
+        <v>93</v>
       </c>
       <c r="C29" t="s">
-        <v>128</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>127</v>
+        <v>205</v>
       </c>
       <c r="B30" t="s">
-        <v>126</v>
+        <v>91</v>
       </c>
       <c r="C30" t="s">
-        <v>125</v>
+        <v>206</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>124</v>
+        <v>90</v>
       </c>
       <c r="B31" t="s">
-        <v>123</v>
+        <v>89</v>
       </c>
       <c r="C31" t="s">
-        <v>122</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>121</v>
+        <v>87</v>
       </c>
       <c r="B32" t="s">
-        <v>120</v>
+        <v>86</v>
       </c>
       <c r="C32" t="s">
-        <v>119</v>
+        <v>85</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
       <c r="B33" t="s">
-        <v>117</v>
+        <v>83</v>
       </c>
       <c r="C33" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="B34" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="C34" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>112</v>
+        <v>78</v>
       </c>
       <c r="B35" t="s">
-        <v>111</v>
+        <v>77</v>
       </c>
       <c r="C35" t="s">
-        <v>110</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>109</v>
+        <v>75</v>
       </c>
       <c r="B36" t="s">
-        <v>108</v>
+        <v>74</v>
       </c>
       <c r="C36" t="s">
-        <v>107</v>
+        <v>73</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>106</v>
+        <v>72</v>
       </c>
       <c r="B37" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
       <c r="C37" t="s">
-        <v>104</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>103</v>
+        <v>168</v>
       </c>
       <c r="B38" t="s">
-        <v>102</v>
+        <v>64</v>
       </c>
       <c r="C38" t="s">
-        <v>101</v>
+        <v>169</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="B39" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="C39" t="s">
-        <v>98</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>97</v>
+        <v>66</v>
       </c>
       <c r="B40" t="s">
-        <v>96</v>
+        <v>167</v>
       </c>
       <c r="C40" t="s">
-        <v>95</v>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>182</v>
+      </c>
+      <c r="B42" t="s">
+        <v>181</v>
+      </c>
+      <c r="C42" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>94</v>
+        <v>172</v>
       </c>
       <c r="B43" t="s">
-        <v>93</v>
+        <v>173</v>
       </c>
       <c r="C43" t="s">
-        <v>92</v>
+        <v>174</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>91</v>
+        <v>62</v>
       </c>
       <c r="B44" t="s">
-        <v>90</v>
+        <v>5</v>
       </c>
       <c r="C44" t="s">
-        <v>89</v>
+        <v>178</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>60</v>
+      </c>
+      <c r="B45" t="s">
+        <v>59</v>
+      </c>
+      <c r="C45" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>88</v>
+        <v>57</v>
       </c>
       <c r="B46" t="s">
-        <v>87</v>
+        <v>56</v>
       </c>
       <c r="C46" t="s">
-        <v>86</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>54</v>
+      </c>
+      <c r="B47" t="s">
+        <v>53</v>
+      </c>
+      <c r="C47" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>85</v>
+        <v>1</v>
       </c>
       <c r="B48" t="s">
-        <v>84</v>
+        <v>0</v>
       </c>
       <c r="C48" t="s">
-        <v>83</v>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>50</v>
+      </c>
+      <c r="B49" t="s">
+        <v>49</v>
+      </c>
+      <c r="C49" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>184</v>
+      </c>
+      <c r="B50" t="s">
+        <v>185</v>
+      </c>
+      <c r="C50" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>82</v>
+        <v>47</v>
       </c>
       <c r="B51" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="C51" t="s">
-        <v>81</v>
+        <v>45</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>80</v>
+        <v>44</v>
       </c>
       <c r="B52" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
       <c r="C52" t="s">
-        <v>78</v>
+        <v>175</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>77</v>
+        <v>39</v>
       </c>
       <c r="B53" t="s">
-        <v>76</v>
+        <v>38</v>
       </c>
       <c r="C53" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>74</v>
+        <v>42</v>
       </c>
       <c r="B54" t="s">
-        <v>73</v>
+        <v>41</v>
       </c>
       <c r="C54" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>71</v>
+        <v>36</v>
       </c>
       <c r="B55" t="s">
-        <v>70</v>
+        <v>35</v>
       </c>
       <c r="C55" t="s">
-        <v>69</v>
+        <v>34</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
       <c r="B56" t="s">
-        <v>67</v>
+        <v>32</v>
       </c>
       <c r="C56" t="s">
-        <v>66</v>
+        <v>176</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="B57" t="s">
-        <v>64</v>
+        <v>29</v>
       </c>
       <c r="C57" t="s">
-        <v>63</v>
+        <v>177</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>62</v>
+        <v>207</v>
       </c>
       <c r="B58" t="s">
         <v>61</v>
       </c>
       <c r="C58" t="s">
-        <v>60</v>
+        <v>208</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="B59" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="C59" t="s">
-        <v>57</v>
+        <v>179</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="B60" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="C60" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="B61" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="C61" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="B62" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="C62" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>47</v>
+        <v>189</v>
       </c>
       <c r="B63" t="s">
-        <v>46</v>
+        <v>190</v>
       </c>
       <c r="C63" t="s">
-        <v>45</v>
+        <v>191</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>44</v>
+        <v>187</v>
       </c>
       <c r="B64" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="C64" t="s">
-        <v>42</v>
+        <v>188</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="B65" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="C65" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="B66" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="C66" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="B67" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="C67" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>32</v>
+        <v>192</v>
       </c>
       <c r="B68" t="s">
-        <v>31</v>
+        <v>201</v>
       </c>
       <c r="C68" t="s">
-        <v>30</v>
+        <v>193</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>29</v>
+        <v>203</v>
       </c>
       <c r="B69" t="s">
-        <v>28</v>
+        <v>209</v>
       </c>
       <c r="C69" t="s">
-        <v>27</v>
+        <v>204</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="B70" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="C70" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>23</v>
-      </c>
-      <c r="B71" t="s">
-        <v>22</v>
-      </c>
-      <c r="C71" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>20</v>
-      </c>
-      <c r="B72" t="s">
-        <v>19</v>
-      </c>
-      <c r="C72" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>17</v>
-      </c>
-      <c r="B73" t="s">
-        <v>16</v>
-      </c>
-      <c r="C73" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>14</v>
-      </c>
-      <c r="B74" t="s">
-        <v>13</v>
-      </c>
-      <c r="C74" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>11</v>
-      </c>
-      <c r="B75" t="s">
-        <v>10</v>
-      </c>
-      <c r="C75" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>8</v>
-      </c>
-      <c r="B76" t="s">
-        <v>7</v>
-      </c>
-      <c r="C76" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>5</v>
-      </c>
-      <c r="B77" t="s">
-        <v>4</v>
-      </c>
-      <c r="C77" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>2</v>
-      </c>
-      <c r="B78" t="s">
-        <v>1</v>
-      </c>
-      <c r="C78" t="s">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
+  <sortState ref="A2:C71">
+    <sortCondition ref="A2"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Concatenate and form with new labels
Added Category:Locations and Category:Series to tables and adjusted the
X-BEDEWORK-PARAM on TOPICAL AREAS sheet to reflect proper capitlization
of series string.
</commit_message>
<xml_diff>
--- a/20140722_TOPICAL_AREAS_SHEET_REVISION.xlsx
+++ b/20140722_TOPICAL_AREAS_SHEET_REVISION.xlsx
@@ -88,9 +88,6 @@
     <t>Snacks</t>
   </si>
   <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Writers Circle:/user/agrp_calsuite-MainCampus/series/Writers Circle</t>
-  </si>
-  <si>
     <t>2a3e9efe-36fd9107-0137-13d788c9-00006c25</t>
   </si>
   <si>
@@ -118,27 +115,18 @@
     <t>series/Salon@615</t>
   </si>
   <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Night at the Library:/user/agrp_calsuite-MainCampus/series/Night at the Library</t>
-  </si>
-  <si>
     <t>ff808181-1fd7389e-011f-d7389f38-00000013</t>
   </si>
   <si>
     <t>series/Night at the Library</t>
   </si>
   <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Nashville Reads:/user/agrp_calsuite-MainCampus/series/Nashville Reads</t>
-  </si>
-  <si>
     <t>2a3e9efe-3c9a9aa5-013c-a71c2016-00006c0b</t>
   </si>
   <si>
     <t>series/Nashville Reads</t>
   </si>
   <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/NCAA:/user/agrp_calsuite-MainCampus/series/NCAA</t>
-  </si>
-  <si>
     <t>2a3e9efe-4135b172-0141-37f8502a-00001779</t>
   </si>
   <si>
@@ -151,18 +139,12 @@
     <t>series/Movies @ Main</t>
   </si>
   <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Move It March:/user/agrp_calsuite-MainCampus/series/Move It March</t>
-  </si>
-  <si>
     <t>2a3e9efe-3c9a9aa5-013c-a72aa11e-00006faf</t>
   </si>
   <si>
     <t>series/Move It March</t>
   </si>
   <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Holiday:/user/agrp_calsuite-MainCampus/series/Holiday</t>
-  </si>
-  <si>
     <t>ff808181-1fd7389e-011f-d7389f47-00000017</t>
   </si>
   <si>
@@ -172,27 +154,18 @@
     <t>2a3e9efe-334bc29f-0133-7a0374b5-000036d0</t>
   </si>
   <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Community of Many Faces:/user/agrp_calsuite-MainCampus/series/Community of Many Faces</t>
-  </si>
-  <si>
     <t>2a3e9efe-35dd67b8-0135-e8e17628-000012e4</t>
   </si>
   <si>
     <t>series/Community of Many Faces</t>
   </si>
   <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Community Cinema:/user/agrp_calsuite-MainCampus/series/Community Cinema</t>
-  </si>
-  <si>
     <t>2a3e9efe-334bc29f-0133-7a022101-000036ce</t>
   </si>
   <si>
     <t>series/Community Cinema</t>
   </si>
   <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Closed:/user/agrp_calsuite-MainCampus/series/Closed</t>
-  </si>
-  <si>
     <t>2a3e9efe-38d85c92-0138-d88f7223-000001ea</t>
   </si>
   <si>
@@ -538,27 +511,6 @@
     <t>2a3e9efe-432e9841-0143-3040dc3a-00000dcb</t>
   </si>
   <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/African American History Month:/user/agrp_calsuite-MainCampus/series/African American History Month</t>
-  </si>
-  <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Movies @ Main:/user/agrp_calsuite-MainCampus/series/Movies @ Main</t>
-  </si>
-  <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Salon@615:/user/agrp_calsuite-MainCampus/series/Salon@615</t>
-  </si>
-  <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Thinking Out of the Lunch Box:/user/agrp_calsuite-MainCampus/series/Thinking Out of the Lunch Box</t>
-  </si>
-  <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Artober:/user/agrp_calsuite-MainCampus/series/Artober</t>
-  </si>
-  <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Wishing Chair Productions:/user/agrp_calsuite-MainCampus/series/Wishing Chair Productions</t>
-  </si>
-  <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Hispanic Heritage Month:/user/agrp_calsuite-MainCampus/series/Hispanic Heritage Month</t>
-  </si>
-  <si>
     <t>ff808181-1fd7389e-011f-d7389ed0-00000002</t>
   </si>
   <si>
@@ -574,9 +526,6 @@
     <t>2a3e9efe-432e9841-0143-303b3a57-00000dad</t>
   </si>
   <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Hunger Awareness:/user/agrp_calsuite-MainCampus/series/Hunger Awareness</t>
-  </si>
-  <si>
     <t>Summer Challenge</t>
   </si>
   <si>
@@ -640,10 +589,61 @@
     <t>series/Virtuoso Showcase Classical Guitar</t>
   </si>
   <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Virtuoso Showcase Classical Guitar:/user/agrp_calsuite-MainCampus/series/Virtuoso Showcase Classical Guitar</t>
-  </si>
-  <si>
     <t>2a3e9ebb-47ca823e-0147-ca9cd657-00000020</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=African American History Month:/user/agrp_calsuite-MainCampus/Series/African American History Month</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Artober:/user/agrp_calsuite-MainCampus/Series/Artober</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Closed:/user/agrp_calsuite-MainCampus/Series/Closed</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Community Cinema:/user/agrp_calsuite-MainCampus/Series/Community Cinema</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Community of Many Faces:/user/agrp_calsuite-MainCampus/Series/Community of Many Faces</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Hispanic Heritage Month:/user/agrp_calsuite-MainCampus/Series/Hispanic Heritage Month</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Holiday:/user/agrp_calsuite-MainCampus/Series/Holiday</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Hunger Awareness:/user/agrp_calsuite-MainCampus/Series/Hunger Awareness</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Move It March:/user/agrp_calsuite-MainCampus/Series/Move It March</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Movies @ Main:/user/agrp_calsuite-MainCampus/Series/Movies @ Main</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Nashville Reads:/user/agrp_calsuite-MainCampus/Series/Nashville Reads</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=NCAA:/user/agrp_calsuite-MainCampus/Series/NCAA</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Night at the Library:/user/agrp_calsuite-MainCampus/Series/Night at the Library</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Salon@615:/user/agrp_calsuite-MainCampus/Series/Salon@615</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Thinking Out of the Lunch Box:/user/agrp_calsuite-MainCampus/Series/Thinking Out of the Lunch Box</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Virtuoso Showcase Classical Guitar:/user/agrp_calsuite-MainCampus/Series/Virtuoso Showcase Classical Guitar</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Wishing Chair Productions:/user/agrp_calsuite-MainCampus/Series/Wishing Chair Productions</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Writers Circle:/user/agrp_calsuite-MainCampus/Series/Writers Circle</t>
   </si>
 </sst>
 </file>
@@ -1002,8 +1002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1014,442 +1014,442 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="B2" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="C2" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B3" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="C3" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="B4" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C4" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C5" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="B6" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C6" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="B7" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="C7" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>197</v>
+        <v>180</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C8" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="B9" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="C9" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
       <c r="B10" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="C10" t="s">
-        <v>196</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="B11" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="C11" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
       <c r="B12" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="C12" t="s">
-        <v>202</v>
+        <v>185</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="B13" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="C13" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="B14" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="C14" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="B15" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="C15" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="B16" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="C16" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B17" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="C17" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="B18" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="C18" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B19" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="C19" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="B20" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C20" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="B21" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="C21" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="B22" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="C22" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B23" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="C23" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B24" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C24" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="B25" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C25" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="B26" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C26" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B27" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="C27" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="B28" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C28" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="B29" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C29" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>205</v>
+        <v>188</v>
       </c>
       <c r="B30" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C30" t="s">
-        <v>206</v>
+        <v>189</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B31" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="C31" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="B32" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="C32" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="B33" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C33" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B34" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C34" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B35" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C35" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B36" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C36" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B37" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C37" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B38" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C38" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B39" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="C39" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B40" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="C40" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1465,68 +1465,68 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="B42" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="C42" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="B43" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="C43" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B44" t="s">
         <v>5</v>
       </c>
       <c r="C44" t="s">
-        <v>178</v>
+        <v>193</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B45" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C45" t="s">
-        <v>58</v>
+        <v>194</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B46" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C46" t="s">
-        <v>55</v>
+        <v>195</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C47" t="s">
-        <v>52</v>
+        <v>196</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1537,139 +1537,139 @@
         <v>0</v>
       </c>
       <c r="C48" t="s">
-        <v>180</v>
+        <v>197</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B49" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C49" t="s">
-        <v>48</v>
+        <v>198</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="B50" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="C50" t="s">
-        <v>186</v>
+        <v>199</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B51" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C51" t="s">
-        <v>45</v>
+        <v>200</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B52" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C52" t="s">
-        <v>175</v>
+        <v>201</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B53" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C53" t="s">
-        <v>37</v>
+        <v>202</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B54" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C54" t="s">
-        <v>40</v>
+        <v>203</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B55" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C55" t="s">
-        <v>34</v>
+        <v>204</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B56" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C56" t="s">
-        <v>176</v>
+        <v>205</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B57" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C57" t="s">
-        <v>177</v>
+        <v>206</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>190</v>
+      </c>
+      <c r="B58" t="s">
+        <v>52</v>
+      </c>
+      <c r="C58" t="s">
         <v>207</v>
-      </c>
-      <c r="B58" t="s">
-        <v>61</v>
-      </c>
-      <c r="C58" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B59" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C59" t="s">
-        <v>179</v>
+        <v>208</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B60" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C60" t="s">
-        <v>24</v>
+        <v>209</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -1696,24 +1696,24 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>189</v>
+        <v>172</v>
       </c>
       <c r="B63" t="s">
-        <v>190</v>
+        <v>173</v>
       </c>
       <c r="C63" t="s">
-        <v>191</v>
+        <v>174</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>187</v>
+        <v>170</v>
       </c>
       <c r="B64" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C64" t="s">
-        <v>188</v>
+        <v>171</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -1751,24 +1751,24 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>192</v>
+        <v>175</v>
       </c>
       <c r="B68" t="s">
-        <v>201</v>
+        <v>184</v>
       </c>
       <c r="C68" t="s">
-        <v>193</v>
+        <v>176</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>203</v>
+        <v>186</v>
       </c>
       <c r="B69" t="s">
-        <v>209</v>
+        <v>191</v>
       </c>
       <c r="C69" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changes in locations reflect current 3.10 titles and labels
</commit_message>
<xml_diff>
--- a/20140722_TOPICAL_AREAS_SHEET_REVISION.xlsx
+++ b/20140722_TOPICAL_AREAS_SHEET_REVISION.xlsx
@@ -1002,8 +1002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added new categories to Topical Areas Sheet
Included newer categories. Updated series to work. Concatenate file
working for 3.10 includes two generic lines for Series and Locations
</commit_message>
<xml_diff>
--- a/20140722_TOPICAL_AREAS_SHEET_REVISION.xlsx
+++ b/20140722_TOPICAL_AREAS_SHEET_REVISION.xlsx
@@ -14,10 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="210">
-  <si>
-    <t>2a3e9efe-40ed9887-0140-ee844b42-000004aa</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="142">
   <si>
     <t>series/Hispanic Heritage Month</t>
   </si>
@@ -25,165 +22,81 @@
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Outreach:/user/agrp_calsuite-MainCampus/Outreach</t>
   </si>
   <si>
-    <t>2a3e9efe-4135b172-0141-37e84116-00001706</t>
-  </si>
-  <si>
     <t>Outreach</t>
   </si>
   <si>
-    <t>2a3e9efe-3948a864-0139-58c00d23-00006346</t>
-  </si>
-  <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Writing:/user/agrp_calsuite-MainCampus/Writing</t>
   </si>
   <si>
-    <t>2a3e9efe-334bc29f-0133-f14f75bc-00001df5</t>
-  </si>
-  <si>
     <t>Writing</t>
   </si>
   <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Teens:/user/agrp_calsuite-MainCampus/Teens</t>
   </si>
   <si>
-    <t>2a3e9efe-334bc29f-0133-79d748a2-000036b0</t>
-  </si>
-  <si>
     <t>Teens</t>
   </si>
   <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Teen Crafts:/user/agrp_calsuite-MainCampus/Teen Crafts</t>
-  </si>
-  <si>
-    <t>2a3e9efe-334bc29f-0133-bc4fcd2f-0000762c</t>
-  </si>
-  <si>
-    <t>Teen Crafts</t>
-  </si>
-  <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=sys/Ongoing:/user/agrp_calsuite-MainCampus/sys/Ongoing</t>
   </si>
   <si>
-    <t>402881e7-25b99d14-0125-b9a50c22-00000002</t>
-  </si>
-  <si>
     <t>sys/Ongoing</t>
   </si>
   <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Story Time:/user/agrp_calsuite-MainCampus/Story Time</t>
   </si>
   <si>
-    <t>402881e6-20a21413-0120-a23e31ea-00000016</t>
-  </si>
-  <si>
     <t>Story Time</t>
   </si>
   <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Snacks:/user/agrp_calsuite-MainCampus/Snacks</t>
   </si>
   <si>
-    <t>2a3e9efe-334bc29f-0133-bc4ef48c-0000762a</t>
-  </si>
-  <si>
     <t>Snacks</t>
   </si>
   <si>
-    <t>2a3e9efe-36fd9107-0137-13d788c9-00006c25</t>
-  </si>
-  <si>
     <t>series/Writers Circle</t>
   </si>
   <si>
-    <t>2a3e9efe-334bc29f-0133-7a00e56f-000036cc</t>
-  </si>
-  <si>
     <t>series/Wishing Chair Productions</t>
   </si>
   <si>
-    <t>2a3e9efe-39249ad8-0139-45fd718a-0000434b</t>
-  </si>
-  <si>
     <t>series/Thinking Out of the Lunch Box</t>
   </si>
   <si>
-    <t>2a3e9efe-3c9a9aa5-013c-a733b8e3-00007021</t>
-  </si>
-  <si>
-    <t>2a3e9efe-334bc29f-0133-7a04041e-000036d1</t>
-  </si>
-  <si>
     <t>series/Salon@615</t>
   </si>
   <si>
-    <t>ff808181-1fd7389e-011f-d7389f38-00000013</t>
-  </si>
-  <si>
     <t>series/Night at the Library</t>
   </si>
   <si>
-    <t>2a3e9efe-3c9a9aa5-013c-a71c2016-00006c0b</t>
-  </si>
-  <si>
     <t>series/Nashville Reads</t>
   </si>
   <si>
-    <t>2a3e9efe-4135b172-0141-37f8502a-00001779</t>
-  </si>
-  <si>
     <t>series/NCAA</t>
   </si>
   <si>
-    <t>2a3e9efe-334bc29f-0133-7a02c06c-000036cf</t>
-  </si>
-  <si>
     <t>series/Movies @ Main</t>
   </si>
   <si>
-    <t>2a3e9efe-3c9a9aa5-013c-a72aa11e-00006faf</t>
-  </si>
-  <si>
     <t>series/Move It March</t>
   </si>
   <si>
-    <t>ff808181-1fd7389e-011f-d7389f47-00000017</t>
-  </si>
-  <si>
     <t>series/Holiday</t>
   </si>
   <si>
-    <t>2a3e9efe-334bc29f-0133-7a0374b5-000036d0</t>
-  </si>
-  <si>
-    <t>2a3e9efe-35dd67b8-0135-e8e17628-000012e4</t>
-  </si>
-  <si>
     <t>series/Community of Many Faces</t>
   </si>
   <si>
-    <t>2a3e9efe-334bc29f-0133-7a022101-000036ce</t>
-  </si>
-  <si>
     <t>series/Community Cinema</t>
   </si>
   <si>
-    <t>2a3e9efe-38d85c92-0138-d88f7223-000001ea</t>
-  </si>
-  <si>
     <t>series/Closed</t>
   </si>
   <si>
-    <t>2a3e9efe-3948a864-0139-58cae8e7-000063e9</t>
-  </si>
-  <si>
     <t>series/Artober</t>
   </si>
   <si>
-    <t>2a3e9efe-34870943-0134-8a28d156-00000286</t>
-  </si>
-  <si>
-    <t>2a3e9efe-334bc29f-0133-f14fd5fa-00001df8</t>
-  </si>
-  <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Music:/user/agrp_calsuite-MainCampus/Music</t>
   </si>
   <si>
@@ -193,264 +106,165 @@
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Movies:/user/agrp_calsuite-MainCampus/Movies</t>
   </si>
   <si>
-    <t>ff808181-1fd7389e-011f-d7389f02-00000005</t>
-  </si>
-  <si>
     <t>Movies</t>
   </si>
   <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Watkins Park:/user/agrp_calsuite-MainCampus/Watkins Park</t>
   </si>
   <si>
-    <t>402881e6-20a21413-0120-a24c742e-00000058</t>
-  </si>
-  <si>
     <t>location/Watkins Park</t>
   </si>
   <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Thompson Lane:/user/agrp_calsuite-MainCampus/Thompson Lane</t>
   </si>
   <si>
-    <t>2a3e9efe-334bc29f-0133-79c130b9-00003696</t>
-  </si>
-  <si>
     <t>location/Thompson Lane</t>
   </si>
   <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Southeast:/user/agrp_calsuite-MainCampus/Southeast</t>
   </si>
   <si>
-    <t>2a3e9efe-334bc29f-0133-79c0df84-00003695</t>
-  </si>
-  <si>
     <t>location/Southeast</t>
   </si>
   <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Richland Park:/user/agrp_calsuite-MainCampus/Richland Park</t>
   </si>
   <si>
-    <t>2a3e9efe-334bc29f-0133-79c02159-00003694</t>
-  </si>
-  <si>
     <t>location/Richland Park</t>
   </si>
   <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Pruitt:/user/agrp_calsuite-MainCampus/Pruitt</t>
   </si>
   <si>
-    <t>2a3e9efe-334bc29f-0133-79bfb656-00003693</t>
-  </si>
-  <si>
     <t>location/Pruitt</t>
   </si>
   <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Old Hickory:/user/agrp_calsuite-MainCampus/Old Hickory</t>
   </si>
   <si>
-    <t>402881e6-20a21413-0120-a24bfbc2-00000057</t>
-  </si>
-  <si>
     <t>location/Old Hickory</t>
   </si>
   <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=North:/user/agrp_calsuite-MainCampus/North</t>
   </si>
   <si>
-    <t>00f1fcb8-20a5687f-0120-a573f575-0000003e</t>
-  </si>
-  <si>
     <t>location/North</t>
   </si>
   <si>
-    <t>ff808181-1fd7389e-011f-d7389fa2-00000028</t>
-  </si>
-  <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Madison:/user/agrp_calsuite-MainCampus/Madison</t>
   </si>
   <si>
-    <t>2a3e9efe-334bc29f-0133-79be9732-00003691</t>
-  </si>
-  <si>
     <t>location/Madison</t>
   </si>
   <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Looby:/user/agrp_calsuite-MainCampus/Looby</t>
   </si>
   <si>
-    <t>402881e6-20a21413-0120-a247d070-0000001f</t>
-  </si>
-  <si>
     <t>location/Looby</t>
   </si>
   <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Inglewood:/user/agrp_calsuite-MainCampus/Inglewood</t>
   </si>
   <si>
-    <t>2a3e9efe-334bc29f-0133-79be1a6a-00003690</t>
-  </si>
-  <si>
     <t>location/Inglewood</t>
   </si>
   <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Hermitage:/user/agrp_calsuite-MainCampus/Hermitage</t>
   </si>
   <si>
-    <t>2a3e9efe-334bc29f-0133-79bdb314-0000368f</t>
-  </si>
-  <si>
     <t>location/Hermitage</t>
   </si>
   <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Hadley Park:/user/agrp_calsuite-MainCampus/Hadley Park</t>
   </si>
   <si>
-    <t>2a3e9efe-334bc29f-0133-79bd46a4-0000368e</t>
-  </si>
-  <si>
     <t>location/Hadley Park</t>
   </si>
   <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Green Hills:/user/agrp_calsuite-MainCampus/Green Hills</t>
   </si>
   <si>
-    <t>2a3e9efe-334bc29f-0133-79bc5a9d-0000368c</t>
-  </si>
-  <si>
     <t>location/Green Hills</t>
   </si>
   <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Goodlettsville:/user/agrp_calsuite-MainCampus/Goodlettsville</t>
   </si>
   <si>
-    <t>2a3e9efe-334bc29f-0133-79bb8e0d-0000368b</t>
-  </si>
-  <si>
     <t>location/Goodlettsville</t>
   </si>
   <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Edmondson Pike:/user/agrp_calsuite-MainCampus/Edmondson Pike</t>
   </si>
   <si>
-    <t>2a3e9efe-334bc29f-0133-79b97775-0000368a</t>
-  </si>
-  <si>
     <t>location/Edmondson Pike</t>
   </si>
   <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Edgehill:/user/agrp_calsuite-MainCampus/Edgehill</t>
   </si>
   <si>
-    <t>2a3e9efe-334bc29f-0133-c7e475fa-0000017e</t>
-  </si>
-  <si>
     <t>location/Edgehill</t>
   </si>
   <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=East:/user/agrp_calsuite-MainCampus/East</t>
   </si>
   <si>
-    <t>402881e6-20a21413-0120-a248f865-00000020</t>
-  </si>
-  <si>
     <t>location/East</t>
   </si>
   <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Donelson:/user/agrp_calsuite-MainCampus/Donelson</t>
   </si>
   <si>
-    <t>2a3e9efe-334bc29f-0133-79b91de3-00003689</t>
-  </si>
-  <si>
     <t>location/Donelson</t>
   </si>
   <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Bordeaux:/user/agrp_calsuite-MainCampus/Bordeaux</t>
   </si>
   <si>
-    <t>2a3e9efe-334bc29f-0133-79b8a609-00003688</t>
-  </si>
-  <si>
     <t>location/Bordeaux</t>
   </si>
   <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Bellevue:/user/agrp_calsuite-MainCampus/Bellevue</t>
   </si>
   <si>
-    <t>2a3e9efe-334bc29f-0133-79b8367c-00003687</t>
-  </si>
-  <si>
     <t>location/Bellevue</t>
   </si>
   <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Jobs:/user/agrp_calsuite-MainCampus/Jobs</t>
   </si>
   <si>
-    <t>2a3e9efe-334bc29f-0133-f15087f5-00001dfb</t>
-  </si>
-  <si>
     <t>Jobs</t>
   </si>
   <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Home and Garden:/user/agrp_calsuite-MainCampus/Home and Garden</t>
   </si>
   <si>
-    <t>2a3e9efe-3ea8ac68-013e-aa095a3d-00001595</t>
-  </si>
-  <si>
     <t>Home and Garden</t>
   </si>
   <si>
-    <t>2a3e9efe-35dd67b8-0135-e8eb41e5-000012f4</t>
-  </si>
-  <si>
-    <t>2a3e9efe-35dd67b8-0135-f8474b67-00005c80</t>
-  </si>
-  <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Exhibits:/user/agrp_calsuite-MainCampus/Exhibits</t>
   </si>
   <si>
-    <t>ff808181-1fd7389e-011f-d7389eff-00000004</t>
-  </si>
-  <si>
     <t>Exhibits</t>
   </si>
   <si>
-    <t>ff808181-1fd7389e-011f-d7389ef9-00000003</t>
-  </si>
-  <si>
-    <t>2a3e9efe-334bc29f-0133-f14ece3f-00001df3</t>
-  </si>
-  <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Children:/user/agrp_calsuite-MainCampus/Children</t>
   </si>
   <si>
-    <t>ff808181-1fd7389e-011f-d7389f33-00000012</t>
-  </si>
-  <si>
     <t>Children</t>
   </si>
   <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Book Clubs:/user/agrp_calsuite-MainCampus/Book Clubs</t>
   </si>
   <si>
-    <t>402881e6-20a21413-0120-a23d71e5-00000015</t>
-  </si>
-  <si>
     <t>Book Clubs</t>
   </si>
   <si>
-    <t>ff808181-1fd73b03-011f-d73b06f8-0000000c</t>
-  </si>
-  <si>
     <t>Arts and Crafts</t>
   </si>
   <si>
     <t>X-BEDEWORK-ALIAS</t>
   </si>
   <si>
-    <t>BEDEWORK TOPICAL AREA CATUID</t>
-  </si>
-  <si>
     <t>TOPICAL AREA LABEL</t>
   </si>
   <si>
@@ -460,9 +274,6 @@
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Author Talks:/user/agrp_calsuite-MainCampus/Author Talks</t>
   </si>
   <si>
-    <t>2a3e9ebb-47c63158-0147-c6315859-00000000</t>
-  </si>
-  <si>
     <t>Computers and Technology</t>
   </si>
   <si>
@@ -484,15 +295,9 @@
     <t>Homework Help</t>
   </si>
   <si>
-    <t>2a3e9efe-334bc29f-0133-f150031d-00001df9</t>
-  </si>
-  <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Homework Help:/user/agrp_calsuite-MainCampus/Homework Help</t>
   </si>
   <si>
-    <t>ff808181-1fd73b03-011f-d73b0642-00000001</t>
-  </si>
-  <si>
     <t>Money and Taxes</t>
   </si>
   <si>
@@ -508,12 +313,6 @@
     <t>series/African American History Month</t>
   </si>
   <si>
-    <t>2a3e9efe-432e9841-0143-3040dc3a-00000dcb</t>
-  </si>
-  <si>
-    <t>ff808181-1fd7389e-011f-d7389ed0-00000002</t>
-  </si>
-  <si>
     <t>Puppet Shows</t>
   </si>
   <si>
@@ -523,9 +322,6 @@
     <t>series/Hunger Awareness</t>
   </si>
   <si>
-    <t>2a3e9efe-432e9841-0143-303b3a57-00000dad</t>
-  </si>
-  <si>
     <t>Summer Challenge</t>
   </si>
   <si>
@@ -535,9 +331,6 @@
     <t>Studio NPL</t>
   </si>
   <si>
-    <t>2a3e9ebb-47ca823e-0147-ca9c67cd-0000001e</t>
-  </si>
-  <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Studio NPL:/user/agrp_calsuite-MainCampus/Studio NPL</t>
   </si>
   <si>
@@ -565,12 +358,6 @@
     <t>First Tuesday at the Archives</t>
   </si>
   <si>
-    <t>2a3e9ebb-47ca823e-0147-ca9bba18-0000001c</t>
-  </si>
-  <si>
-    <t>2a3e9ebb-47ca823e-0147-ca9c9c61-0000001f</t>
-  </si>
-  <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=First Tuesday at the Archives:/user/agrp_calsuite-MainCampus/First Tuesday at the Archives</t>
   </si>
   <si>
@@ -589,61 +376,70 @@
     <t>series/Virtuoso Showcase Classical Guitar</t>
   </si>
   <si>
-    <t>2a3e9ebb-47ca823e-0147-ca9cd657-00000020</t>
-  </si>
-  <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=African American History Month:/user/agrp_calsuite-MainCampus/Series/African American History Month</t>
-  </si>
-  <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Artober:/user/agrp_calsuite-MainCampus/Series/Artober</t>
-  </si>
-  <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Closed:/user/agrp_calsuite-MainCampus/Series/Closed</t>
-  </si>
-  <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Community Cinema:/user/agrp_calsuite-MainCampus/Series/Community Cinema</t>
-  </si>
-  <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Community of Many Faces:/user/agrp_calsuite-MainCampus/Series/Community of Many Faces</t>
-  </si>
-  <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Hispanic Heritage Month:/user/agrp_calsuite-MainCampus/Series/Hispanic Heritage Month</t>
-  </si>
-  <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Holiday:/user/agrp_calsuite-MainCampus/Series/Holiday</t>
-  </si>
-  <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Hunger Awareness:/user/agrp_calsuite-MainCampus/Series/Hunger Awareness</t>
-  </si>
-  <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Move It March:/user/agrp_calsuite-MainCampus/Series/Move It March</t>
-  </si>
-  <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Movies @ Main:/user/agrp_calsuite-MainCampus/Series/Movies @ Main</t>
-  </si>
-  <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Nashville Reads:/user/agrp_calsuite-MainCampus/Series/Nashville Reads</t>
-  </si>
-  <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=NCAA:/user/agrp_calsuite-MainCampus/Series/NCAA</t>
-  </si>
-  <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Night at the Library:/user/agrp_calsuite-MainCampus/Series/Night at the Library</t>
-  </si>
-  <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Salon@615:/user/agrp_calsuite-MainCampus/Series/Salon@615</t>
-  </si>
-  <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Thinking Out of the Lunch Box:/user/agrp_calsuite-MainCampus/Series/Thinking Out of the Lunch Box</t>
-  </si>
-  <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Virtuoso Showcase Classical Guitar:/user/agrp_calsuite-MainCampus/Series/Virtuoso Showcase Classical Guitar</t>
-  </si>
-  <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Wishing Chair Productions:/user/agrp_calsuite-MainCampus/Series/Wishing Chair Productions</t>
-  </si>
-  <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Writers Circle:/user/agrp_calsuite-MainCampus/Series/Writers Circle</t>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/African American History Month:/user/agrp_calsuite-MainCampus/Series/African American History Month</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Community Cinema:/user/agrp_calsuite-MainCampus/Series/Community Cinema</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Community of Many Faces:/user/agrp_calsuite-MainCampus/Series/Community of Many Faces</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Hispanic Heritage Month:/user/agrp_calsuite-MainCampus/Series/Hispanic Heritage Month</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Holiday:/user/agrp_calsuite-MainCampus/Series/Holiday</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Hunger Awareness:/user/agrp_calsuite-MainCampus/Series/Hunger Awareness</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Closed:/user/agrp_calsuite-MainCampus/Series/Closed</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Artober:/user/agrp_calsuite-MainCampus/Series/Artober</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Move It March:/user/agrp_calsuite-MainCampus/Series/Move It March</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Movies @ Main:/user/agrp_calsuite-MainCampus/Series/Movies @ Main</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Nashville Reads:/user/agrp_calsuite-MainCampus/Series/Nashville Reads</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/NCAA:/user/agrp_calsuite-MainCampus/Series/NCAA</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Night at the Library:/user/agrp_calsuite-MainCampus/Series/Night at the Library</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Salon@615:/user/agrp_calsuite-MainCampus/Series/Salon@615</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Thinking Out of the Lunch Box:/user/agrp_calsuite-MainCampus/Series/Thinking Out of the Lunch Box</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=seriesVirtuoso Showcase Classical Guitar:/user/agrp_calsuite-MainCampus/Series/Virtuoso Showcase Classical Guitar</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Wishing Chair Productions:/user/agrp_calsuite-MainCampus/Series/Wishing Chair Productions</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Writers Circle:/user/agrp_calsuite-MainCampus/Series/Writers Circle</t>
+  </si>
+  <si>
+    <t>series/Community</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Community:/user/agrp_calsuite-MainCampus/series/Community</t>
+  </si>
+  <si>
+    <t>series/Summer Reading</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Summer Reading:/user/agrp_calsuite-MainCampus/series/Summer Reading</t>
   </si>
 </sst>
 </file>
@@ -1000,10 +796,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C70"/>
+  <dimension ref="A1:C73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1014,772 +810,579 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>144</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
-        <v>143</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>142</v>
-      </c>
-      <c r="B2" t="s">
-        <v>148</v>
+        <v>81</v>
       </c>
       <c r="C2" t="s">
-        <v>177</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>146</v>
-      </c>
-      <c r="B3" t="s">
-        <v>141</v>
+        <v>84</v>
       </c>
       <c r="C3" t="s">
-        <v>147</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>140</v>
-      </c>
-      <c r="B4" t="s">
-        <v>139</v>
+        <v>80</v>
       </c>
       <c r="C4" t="s">
-        <v>138</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>161</v>
-      </c>
-      <c r="B5" t="s">
-        <v>54</v>
+        <v>96</v>
       </c>
       <c r="C5" t="s">
-        <v>162</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>137</v>
-      </c>
-      <c r="B6" t="s">
-        <v>136</v>
+        <v>78</v>
       </c>
       <c r="C6" t="s">
-        <v>135</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>149</v>
-      </c>
-      <c r="B7" t="s">
-        <v>134</v>
+        <v>86</v>
       </c>
       <c r="C7" t="s">
-        <v>150</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>180</v>
-      </c>
-      <c r="B8" t="s">
-        <v>45</v>
+        <v>111</v>
       </c>
       <c r="C8" t="s">
-        <v>181</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>151</v>
-      </c>
-      <c r="B9" t="s">
-        <v>133</v>
+        <v>88</v>
       </c>
       <c r="C9" t="s">
-        <v>152</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>178</v>
-      </c>
-      <c r="B10" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="C10" t="s">
-        <v>179</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>132</v>
-      </c>
-      <c r="B11" t="s">
-        <v>131</v>
+        <v>76</v>
       </c>
       <c r="C11" t="s">
-        <v>130</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>182</v>
-      </c>
-      <c r="B12" t="s">
-        <v>183</v>
+        <v>113</v>
       </c>
       <c r="C12" t="s">
-        <v>185</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>153</v>
-      </c>
-      <c r="B13" t="s">
-        <v>128</v>
+        <v>90</v>
       </c>
       <c r="C13" t="s">
-        <v>154</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>127</v>
-      </c>
-      <c r="B14" t="s">
-        <v>126</v>
+        <v>74</v>
       </c>
       <c r="C14" t="s">
-        <v>125</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>155</v>
-      </c>
-      <c r="B15" t="s">
-        <v>156</v>
+        <v>92</v>
       </c>
       <c r="C15" t="s">
-        <v>157</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>124</v>
-      </c>
-      <c r="B16" t="s">
-        <v>123</v>
+        <v>72</v>
       </c>
       <c r="C16" t="s">
-        <v>122</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>121</v>
-      </c>
-      <c r="B17" t="s">
-        <v>120</v>
+        <v>70</v>
       </c>
       <c r="C17" t="s">
-        <v>119</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>118</v>
-      </c>
-      <c r="B18" t="s">
-        <v>117</v>
+        <v>68</v>
       </c>
       <c r="C18" t="s">
-        <v>116</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>115</v>
-      </c>
-      <c r="B19" t="s">
-        <v>114</v>
+        <v>66</v>
       </c>
       <c r="C19" t="s">
-        <v>113</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>112</v>
-      </c>
-      <c r="B20" t="s">
-        <v>111</v>
+        <v>64</v>
       </c>
       <c r="C20" t="s">
-        <v>110</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>109</v>
-      </c>
-      <c r="B21" t="s">
-        <v>108</v>
+        <v>62</v>
       </c>
       <c r="C21" t="s">
-        <v>107</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>106</v>
-      </c>
-      <c r="B22" t="s">
-        <v>105</v>
+        <v>60</v>
       </c>
       <c r="C22" t="s">
-        <v>104</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>103</v>
-      </c>
-      <c r="B23" t="s">
-        <v>102</v>
+        <v>58</v>
       </c>
       <c r="C23" t="s">
-        <v>101</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>100</v>
-      </c>
-      <c r="B24" t="s">
-        <v>99</v>
+        <v>56</v>
       </c>
       <c r="C24" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>97</v>
-      </c>
-      <c r="B25" t="s">
-        <v>96</v>
+        <v>54</v>
       </c>
       <c r="C25" t="s">
-        <v>95</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>94</v>
-      </c>
-      <c r="B26" t="s">
-        <v>93</v>
+        <v>52</v>
       </c>
       <c r="C26" t="s">
-        <v>92</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>91</v>
-      </c>
-      <c r="B27" t="s">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="C27" t="s">
-        <v>89</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>88</v>
-      </c>
-      <c r="B28" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="C28" t="s">
-        <v>86</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>85</v>
-      </c>
-      <c r="B29" t="s">
-        <v>84</v>
+        <v>46</v>
       </c>
       <c r="C29" t="s">
-        <v>83</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>188</v>
-      </c>
-      <c r="B30" t="s">
-        <v>82</v>
+        <v>117</v>
       </c>
       <c r="C30" t="s">
-        <v>189</v>
+        <v>118</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>81</v>
-      </c>
-      <c r="B31" t="s">
-        <v>80</v>
+        <v>44</v>
       </c>
       <c r="C31" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>78</v>
-      </c>
-      <c r="B32" t="s">
-        <v>77</v>
+        <v>42</v>
       </c>
       <c r="C32" t="s">
-        <v>76</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>75</v>
-      </c>
-      <c r="B33" t="s">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="C33" t="s">
-        <v>73</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>72</v>
-      </c>
-      <c r="B34" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="C34" t="s">
-        <v>70</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>69</v>
-      </c>
-      <c r="B35" t="s">
-        <v>68</v>
+        <v>36</v>
       </c>
       <c r="C35" t="s">
-        <v>67</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>66</v>
-      </c>
-      <c r="B36" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="C36" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>63</v>
-      </c>
-      <c r="B37" t="s">
-        <v>62</v>
+        <v>32</v>
       </c>
       <c r="C37" t="s">
-        <v>61</v>
+        <v>31</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>159</v>
-      </c>
-      <c r="B38" t="s">
-        <v>55</v>
+        <v>94</v>
       </c>
       <c r="C38" t="s">
-        <v>160</v>
+        <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>60</v>
-      </c>
-      <c r="B39" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="C39" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>57</v>
-      </c>
-      <c r="B40" t="s">
-        <v>158</v>
+        <v>28</v>
       </c>
       <c r="C40" t="s">
-        <v>56</v>
+        <v>27</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>4</v>
-      </c>
-      <c r="B41" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C41" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>166</v>
-      </c>
-      <c r="B42" t="s">
-        <v>165</v>
+        <v>99</v>
       </c>
       <c r="C42" t="s">
-        <v>167</v>
+        <v>100</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>163</v>
-      </c>
-      <c r="B43" t="s">
-        <v>164</v>
+        <v>98</v>
       </c>
       <c r="C43" t="s">
-        <v>192</v>
+        <v>120</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>53</v>
-      </c>
-      <c r="B44" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="C44" t="s">
-        <v>193</v>
+        <v>127</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>51</v>
-      </c>
-      <c r="B45" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="C45" t="s">
-        <v>194</v>
+        <v>126</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>49</v>
-      </c>
-      <c r="B46" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="C46" t="s">
-        <v>195</v>
+        <v>121</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>47</v>
-      </c>
-      <c r="B47" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="C47" t="s">
-        <v>196</v>
+        <v>122</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>1</v>
-      </c>
-      <c r="B48" t="s">
         <v>0</v>
       </c>
       <c r="C48" t="s">
-        <v>197</v>
+        <v>123</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>44</v>
-      </c>
-      <c r="B49" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="C49" t="s">
-        <v>198</v>
+        <v>124</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>168</v>
-      </c>
-      <c r="B50" t="s">
-        <v>169</v>
+        <v>101</v>
       </c>
       <c r="C50" t="s">
-        <v>199</v>
+        <v>125</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>42</v>
-      </c>
-      <c r="B51" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="C51" t="s">
-        <v>200</v>
+        <v>128</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>40</v>
-      </c>
-      <c r="B52" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="C52" t="s">
-        <v>201</v>
+        <v>129</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>36</v>
-      </c>
-      <c r="B53" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="C53" t="s">
-        <v>202</v>
+        <v>130</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>38</v>
-      </c>
-      <c r="B54" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="C54" t="s">
-        <v>203</v>
+        <v>131</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>34</v>
-      </c>
-      <c r="B55" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="C55" t="s">
-        <v>204</v>
+        <v>132</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>32</v>
-      </c>
-      <c r="B56" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="C56" t="s">
-        <v>205</v>
+        <v>133</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>29</v>
-      </c>
-      <c r="B57" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="C57" t="s">
-        <v>206</v>
+        <v>134</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>190</v>
-      </c>
-      <c r="B58" t="s">
-        <v>52</v>
+        <v>119</v>
       </c>
       <c r="C58" t="s">
-        <v>207</v>
+        <v>135</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>27</v>
-      </c>
-      <c r="B59" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C59" t="s">
-        <v>208</v>
+        <v>136</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>25</v>
-      </c>
-      <c r="B60" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C60" t="s">
-        <v>209</v>
+        <v>137</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>23</v>
-      </c>
-      <c r="B61" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C61" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>20</v>
-      </c>
-      <c r="B62" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C62" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>172</v>
-      </c>
-      <c r="B63" t="s">
-        <v>173</v>
+        <v>104</v>
       </c>
       <c r="C63" t="s">
-        <v>174</v>
+        <v>105</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>170</v>
-      </c>
-      <c r="B64" t="s">
-        <v>30</v>
+        <v>102</v>
       </c>
       <c r="C64" t="s">
-        <v>171</v>
+        <v>103</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>17</v>
-      </c>
-      <c r="B65" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C65" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>14</v>
-      </c>
-      <c r="B66" t="s">
-        <v>13</v>
-      </c>
-      <c r="C66" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>11</v>
-      </c>
-      <c r="B67" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C67" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>175</v>
-      </c>
-      <c r="B68" t="s">
-        <v>184</v>
+        <v>106</v>
       </c>
       <c r="C68" t="s">
-        <v>176</v>
+        <v>107</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>186</v>
-      </c>
-      <c r="B69" t="s">
-        <v>191</v>
+        <v>115</v>
       </c>
       <c r="C69" t="s">
-        <v>187</v>
+        <v>116</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>8</v>
-      </c>
-      <c r="B70" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C70" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>2</v>
+      </c>
+      <c r="C71" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>138</v>
+      </c>
+      <c r="C72" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>140</v>
+      </c>
+      <c r="C73" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed outdated categories, add new
Made sure all the capitalization and language exactly matches the
current categories as programmed into 3.10 for sorting on the public
interface,
</commit_message>
<xml_diff>
--- a/20140722_TOPICAL_AREAS_SHEET_REVISION.xlsx
+++ b/20140722_TOPICAL_AREAS_SHEET_REVISION.xlsx
@@ -14,13 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="198">
-  <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Outreach:/user/agrp_calsuite-MainCampus/Outreach</t>
-  </si>
-  <si>
-    <t>Outreach</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="199">
   <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Writing:/user/agrp_calsuite-MainCampus/Writing</t>
   </si>
@@ -34,12 +28,6 @@
     <t>Teens</t>
   </si>
   <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=sys/Ongoing:/user/agrp_calsuite-MainCampus/sys/Ongoing</t>
-  </si>
-  <si>
-    <t>sys/Ongoing</t>
-  </si>
-  <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Story Time:/user/agrp_calsuite-MainCampus/Story Time</t>
   </si>
   <si>
@@ -253,12 +241,6 @@
     <t>TOPICAL AREA LABEL</t>
   </si>
   <si>
-    <t>series/Community</t>
-  </si>
-  <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Community:/user/agrp_calsuite-MainCampus/series/Community</t>
-  </si>
-  <si>
     <t>BEDEWORK TOPICAL AREA CATUID</t>
   </si>
   <si>
@@ -268,15 +250,9 @@
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Arts &amp; Crafts:/user/agrp_calsuite-MainCampus/Arts &amp; Crafts</t>
   </si>
   <si>
-    <t>Authors</t>
-  </si>
-  <si>
     <t>ff808181-1fd73b03-011f-d73b06f8-0000000c</t>
   </si>
   <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Authors:/user/agrp_calsuite-MainCampus/Authors</t>
-  </si>
-  <si>
     <t>402881e6-20a21413-0120-a23d71e5-00000015</t>
   </si>
   <si>
@@ -292,45 +268,18 @@
     <t>ff808181-1fd7389e-011f-d7389f33-00000012</t>
   </si>
   <si>
-    <t>Computers</t>
-  </si>
-  <si>
     <t>2a3e9efe-334bc29f-0133-f14ece3f-00001df3</t>
   </si>
   <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Computers:/user/agrp_calsuite-MainCampus/Computers</t>
-  </si>
-  <si>
-    <t>Dance</t>
-  </si>
-  <si>
     <t>ff808181-1fd7389e-011f-d7389ef9-00000003</t>
   </si>
   <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Dance:/user/agrp_calsuite-MainCampus/Dance</t>
-  </si>
-  <si>
     <t>ff808181-1fd7389e-011f-d7389eff-00000004</t>
   </si>
   <si>
-    <t>Featured</t>
-  </si>
-  <si>
-    <t>2a3e9efe-35dd67b8-0135-f8474b67-00005c80</t>
-  </si>
-  <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Featured:/user/agrp_calsuite-MainCampus/Featured</t>
-  </si>
-  <si>
-    <t>Health</t>
-  </si>
-  <si>
     <t>2a3e9efe-35dd67b8-0135-e8eb41e5-000012f4</t>
   </si>
   <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Health:/user/agrp_calsuite-MainCampus/Health</t>
-  </si>
-  <si>
     <t>2a3e9efe-3ea8ac68-013e-aa095a3d-00001595</t>
   </si>
   <si>
@@ -376,24 +325,12 @@
     <t>2a3e9efe-334bc29f-0133-79be9732-00003691</t>
   </si>
   <si>
-    <t>location/Main</t>
-  </si>
-  <si>
     <t>ff808181-1fd7389e-011f-d7389fa2-00000028</t>
   </si>
   <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=MAIN:/user/agrp_calsuite-MainCampus/Locations/MAIN</t>
   </si>
   <si>
-    <t>location/Metro Archives</t>
-  </si>
-  <si>
-    <t>2a3e9efe-334bc29f-0133-79befbc0-00003692</t>
-  </si>
-  <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Metro Archives:/user/agrp_calsuite-MainCampus/Metro Archives</t>
-  </si>
-  <si>
     <t>00f1fcb8-20a5687f-0120-a573f575-0000003e</t>
   </si>
   <si>
@@ -427,24 +364,12 @@
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Music:/user/agrp_calsuite-MainCampus/Music</t>
   </si>
   <si>
-    <t>Personal Finance</t>
-  </si>
-  <si>
     <t>2a3e9efe-334bc29f-0133-f14fd5fa-00001df8</t>
   </si>
   <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Personal Finance:/user/agrp_calsuite-MainCampus/Personal Finance</t>
-  </si>
-  <si>
-    <t>Sale</t>
-  </si>
-  <si>
     <t>2a3e9efe-34870943-0134-8a28d156-00000286</t>
   </si>
   <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Sale:/user/agrp_calsuite-MainCampus/Sale</t>
-  </si>
-  <si>
     <t>Series</t>
   </si>
   <si>
@@ -457,18 +382,9 @@
     <t>2a3e9efe-3948a864-0139-58c00d23-00006346</t>
   </si>
   <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Artober:/user/agrp_calsuite-MainCampus/Series/Artober</t>
-  </si>
-  <si>
-    <t>series/Classical Guitar</t>
-  </si>
-  <si>
     <t>2a3e9efe-3948a864-0139-58cae8e7-000063e9</t>
   </si>
   <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Classical Guitar:/user/agrp_calsuite-MainCampus/series/Classical Guitar</t>
-  </si>
-  <si>
     <t>2a3e9efe-38d85c92-0138-d88f7223-000001ea</t>
   </si>
   <si>
@@ -538,21 +454,12 @@
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Salon@615:/user/agrp_calsuite-MainCampus/series/Salon@615</t>
   </si>
   <si>
-    <t>series/Summer Reading</t>
-  </si>
-  <si>
     <t>2a3e9efe-3c9a9aa5-013c-a733b8e3-00007021</t>
   </si>
   <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Summer Reading:/user/agrp_calsuite-MainCampus/series/Summer Reading</t>
-  </si>
-  <si>
     <t>2a3e9efe-39249ad8-0139-45fd718a-0000434b</t>
   </si>
   <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Thinking Out of the Lunch Box:/user/agrp_calsuite-MainCampus/Series/Thinking Out of the Lunch Box</t>
-  </si>
-  <si>
     <t>2a3e9efe-334bc29f-0133-7a00e56f-000036cc</t>
   </si>
   <si>
@@ -565,21 +472,9 @@
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Writers Circle:/user/agrp_calsuite-MainCampus/series/Writers Circle</t>
   </si>
   <si>
-    <t>Snacks</t>
-  </si>
-  <si>
-    <t>2a3e9efe-334bc29f-0133-bc4ef48c-0000762a</t>
-  </si>
-  <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Snacks:/user/agrp_calsuite-MainCampus/Snacks</t>
-  </si>
-  <si>
     <t>402881e6-20a21413-0120-a23e31ea-00000016</t>
   </si>
   <si>
-    <t>402881e7-25b99d14-0125-b9a50c22-00000002</t>
-  </si>
-  <si>
     <t>Teen Crafts</t>
   </si>
   <si>
@@ -592,22 +487,130 @@
     <t>2a3e9efe-334bc29f-0133-79d748a2-000036b0</t>
   </si>
   <si>
-    <t>Theater</t>
-  </si>
-  <si>
-    <t>ff808181-1fd73b03-011f-d73b065c-00000002</t>
-  </si>
-  <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Theater:/user/agrp_calsuite-MainCampus/Theater</t>
-  </si>
-  <si>
     <t>2a3e9efe-334bc29f-0133-f14f75bc-00001df5</t>
   </si>
   <si>
-    <t>2a3e9efe-4135b172-0141-37e84116-00001706</t>
-  </si>
-  <si>
-    <t>2a3e9efe-4135b172-0141-3803bdaa-0000194d</t>
+    <t>Author Talks</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Author Talks:/user/agrp_calsuite-MainCampus/Browse By Topic/Author Talks</t>
+  </si>
+  <si>
+    <t>series/Hunger Awareness</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Hunger Awareness:/user/agrp_calsuite-MainCampus/series/Hunger Awareness</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Book Sales:/user/agrp_calsuite-MainCampus/Book Sales</t>
+  </si>
+  <si>
+    <t>Book Sales</t>
+  </si>
+  <si>
+    <t>Computers and Technology</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Computers and Technology:/user/agrp_calsuite-MainCampus/Computers and Technology</t>
+  </si>
+  <si>
+    <t>Dance and Theater</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Dance and Theater:/user/agrp_calsuite-MainCampus/Dance and Theater</t>
+  </si>
+  <si>
+    <t>ESL</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=ESL:/user/agrp_calsuite-MainCampus/ESL</t>
+  </si>
+  <si>
+    <t>Health and Wellness</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Health and Wellness:/user/agrp_calsuite-MainCampus/Health and Wellness</t>
+  </si>
+  <si>
+    <t>History and Genealogy</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=History and Genealogy:/user/agrp_calsuite-MainCampus/History and Genealogy</t>
+  </si>
+  <si>
+    <t>Homework Help</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Homework Help:/user/agrp_calsuite-MainCampus/Homework Help</t>
+  </si>
+  <si>
+    <t>location/Main Library</t>
+  </si>
+  <si>
+    <t>Money and Taxes</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Money and Taxes:/user/agrp_calsuite-MainCampus/Money and Taxes</t>
+  </si>
+  <si>
+    <t>Puppet Shows</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Puppet Shows:/user/agrp_calsuite-MainCampus/Puppet Shows</t>
+  </si>
+  <si>
+    <t>series/Board Meetings</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Board Meetings:/user/agrp_calsuite-MainCampus/series/Board Meetings</t>
+  </si>
+  <si>
+    <t>series/Hispanic Heritage Month</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Hispanic Heritage Month:/user/agrp_calsuite-MainCampus/series/Hispanic Heritage Month</t>
+  </si>
+  <si>
+    <t>series/Summer Challenge</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Summer Challenge:/user/agrp_calsuite-MainCampus/series/Summer Challenge</t>
+  </si>
+  <si>
+    <t>Small Business</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Small Business:/user/agrp_calsuite-MainCampus/series/Small Business</t>
+  </si>
+  <si>
+    <t>series/TOTAL</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/TOTAL:/user/agrp_calsuite-MainCampus/series/TOTAL</t>
+  </si>
+  <si>
+    <t>series/Virtuoso Showcase Classical Guitar</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Virtuoso Showcase Classical Guitar:/user/agrp_calsuite-MainCampus/series/Virtuoso Showcase Classical Guitar</t>
+  </si>
+  <si>
+    <t>Test Prep</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Test Prep:/user/agrp_calsuite-MainCampus/Test Prep</t>
+  </si>
+  <si>
+    <t>series/Seed Exchange</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Seed Exchange:/user/agrp_calsuite-MainCampus/series/Seed Exchange</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Thinking Out of the Lunch Box:/user/agrp_calsuite-MainCampus/series/Thinking Out of the Lunch Box</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Artober:/user/agrp_calsuite-MainCampus/series/Artober</t>
   </si>
 </sst>
 </file>
@@ -964,10 +967,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C67"/>
+  <dimension ref="A1:C70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -978,145 +981,139 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
         <v>76</v>
       </c>
-      <c r="B2" t="s">
-        <v>82</v>
-      </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>158</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C3" t="s">
-        <v>86</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>163</v>
       </c>
       <c r="B5" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C5" t="s">
-        <v>90</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="C6" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="B7" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="C7" t="s">
-        <v>94</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>164</v>
       </c>
       <c r="B8" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="C8" t="s">
-        <v>97</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>71</v>
+        <v>166</v>
       </c>
       <c r="B9" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="C9" t="s">
-        <v>70</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>99</v>
-      </c>
-      <c r="B10" t="s">
-        <v>100</v>
+        <v>168</v>
       </c>
       <c r="C10" t="s">
-        <v>101</v>
+        <v>169</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>102</v>
+        <v>67</v>
       </c>
       <c r="B11" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C11" t="s">
-        <v>104</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>69</v>
+        <v>170</v>
       </c>
       <c r="B12" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="C12" t="s">
-        <v>68</v>
+        <v>171</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>67</v>
-      </c>
-      <c r="B13" t="s">
-        <v>106</v>
+        <v>172</v>
       </c>
       <c r="C13" t="s">
-        <v>66</v>
+        <v>173</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1124,7 +1121,7 @@
         <v>65</v>
       </c>
       <c r="B14" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="C14" t="s">
         <v>64</v>
@@ -1132,178 +1129,175 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>63</v>
-      </c>
-      <c r="B15" t="s">
-        <v>108</v>
+        <v>174</v>
       </c>
       <c r="C15" t="s">
-        <v>62</v>
+        <v>175</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B16" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="C16" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B17" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="C17" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B18" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B19" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="C19" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B20" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="C20" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B21" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="C21" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="C22" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B23" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="C23" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B24" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
       <c r="C24" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B25" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="C25" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B26" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="C26" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>120</v>
+        <v>41</v>
       </c>
       <c r="B27" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="C27" t="s">
-        <v>122</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>123</v>
+        <v>39</v>
       </c>
       <c r="B28" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="C28" t="s">
-        <v>125</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B29" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
       <c r="C29" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>37</v>
+        <v>176</v>
       </c>
       <c r="B30" t="s">
-        <v>127</v>
+        <v>103</v>
       </c>
       <c r="C30" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1311,7 +1305,7 @@
         <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="C31" t="s">
         <v>34</v>
@@ -1322,7 +1316,7 @@
         <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>129</v>
+        <v>106</v>
       </c>
       <c r="C32" t="s">
         <v>32</v>
@@ -1333,7 +1327,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
       <c r="C33" t="s">
         <v>30</v>
@@ -1344,7 +1338,7 @@
         <v>29</v>
       </c>
       <c r="B34" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="C34" t="s">
         <v>28</v>
@@ -1355,7 +1349,7 @@
         <v>27</v>
       </c>
       <c r="B35" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="C35" t="s">
         <v>26</v>
@@ -1366,7 +1360,7 @@
         <v>25</v>
       </c>
       <c r="B36" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="C36" t="s">
         <v>24</v>
@@ -1374,288 +1368,270 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>134</v>
+        <v>23</v>
       </c>
       <c r="B37" t="s">
-        <v>135</v>
+        <v>111</v>
       </c>
       <c r="C37" t="s">
-        <v>136</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>1</v>
+        <v>177</v>
       </c>
       <c r="B38" t="s">
-        <v>196</v>
+        <v>116</v>
       </c>
       <c r="C38" t="s">
-        <v>0</v>
+        <v>178</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>137</v>
+        <v>21</v>
       </c>
       <c r="B39" t="s">
-        <v>138</v>
+        <v>112</v>
       </c>
       <c r="C39" t="s">
-        <v>139</v>
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>140</v>
+        <v>113</v>
       </c>
       <c r="B40" t="s">
-        <v>141</v>
+        <v>114</v>
       </c>
       <c r="C40" t="s">
-        <v>142</v>
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>143</v>
-      </c>
-      <c r="B41" t="s">
-        <v>144</v>
+        <v>179</v>
       </c>
       <c r="C41" t="s">
-        <v>145</v>
+        <v>180</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>23</v>
+        <v>118</v>
       </c>
       <c r="B42" t="s">
-        <v>146</v>
+        <v>119</v>
       </c>
       <c r="C42" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>148</v>
+        <v>19</v>
       </c>
       <c r="B43" t="s">
-        <v>149</v>
+        <v>121</v>
       </c>
       <c r="C43" t="s">
-        <v>150</v>
+        <v>198</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>22</v>
-      </c>
-      <c r="B44" t="s">
-        <v>151</v>
+        <v>181</v>
       </c>
       <c r="C44" t="s">
-        <v>152</v>
+        <v>182</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>79</v>
+        <v>18</v>
       </c>
       <c r="B45" t="s">
-        <v>197</v>
+        <v>123</v>
       </c>
       <c r="C45" t="s">
-        <v>80</v>
+        <v>124</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B46" t="s">
-        <v>153</v>
+        <v>125</v>
       </c>
       <c r="C46" t="s">
-        <v>154</v>
+        <v>126</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B47" t="s">
-        <v>155</v>
+        <v>127</v>
       </c>
       <c r="C47" t="s">
-        <v>156</v>
+        <v>128</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>157</v>
+        <v>129</v>
       </c>
       <c r="B48" t="s">
-        <v>158</v>
+        <v>130</v>
       </c>
       <c r="C48" t="s">
-        <v>159</v>
+        <v>131</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>19</v>
-      </c>
-      <c r="B49" t="s">
-        <v>160</v>
+        <v>183</v>
       </c>
       <c r="C49" t="s">
-        <v>161</v>
+        <v>184</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B50" t="s">
-        <v>162</v>
+        <v>132</v>
       </c>
       <c r="C50" t="s">
-        <v>163</v>
+        <v>133</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>17</v>
-      </c>
-      <c r="B51" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C51" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B52" t="s">
-        <v>168</v>
+        <v>134</v>
       </c>
       <c r="C52" t="s">
-        <v>169</v>
+        <v>135</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B53" t="s">
-        <v>166</v>
+        <v>136</v>
       </c>
       <c r="C53" t="s">
-        <v>167</v>
+        <v>137</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B54" t="s">
-        <v>170</v>
+        <v>140</v>
       </c>
       <c r="C54" t="s">
-        <v>171</v>
+        <v>141</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B55" t="s">
-        <v>172</v>
+        <v>138</v>
       </c>
       <c r="C55" t="s">
-        <v>173</v>
+        <v>139</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>174</v>
+        <v>10</v>
       </c>
       <c r="B56" t="s">
-        <v>175</v>
+        <v>142</v>
       </c>
       <c r="C56" t="s">
-        <v>176</v>
+        <v>143</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>174</v>
+        <v>9</v>
       </c>
       <c r="B57" t="s">
-        <v>175</v>
+        <v>144</v>
       </c>
       <c r="C57" t="s">
-        <v>176</v>
+        <v>145</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>12</v>
-      </c>
-      <c r="B58" t="s">
-        <v>177</v>
+        <v>195</v>
       </c>
       <c r="C58" t="s">
-        <v>178</v>
+        <v>196</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>11</v>
+        <v>185</v>
       </c>
       <c r="B59" t="s">
-        <v>179</v>
+        <v>146</v>
       </c>
       <c r="C59" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B60" t="s">
-        <v>181</v>
+        <v>147</v>
       </c>
       <c r="C60" t="s">
-        <v>182</v>
+        <v>197</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>183</v>
-      </c>
-      <c r="B61" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="C61" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>9</v>
+        <v>191</v>
       </c>
       <c r="B62" t="s">
-        <v>186</v>
+        <v>122</v>
       </c>
       <c r="C62" t="s">
-        <v>8</v>
+        <v>192</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -1663,58 +1639,85 @@
         <v>7</v>
       </c>
       <c r="B63" t="s">
-        <v>187</v>
+        <v>148</v>
       </c>
       <c r="C63" t="s">
-        <v>6</v>
+        <v>149</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>188</v>
+        <v>6</v>
       </c>
       <c r="B64" t="s">
-        <v>189</v>
+        <v>150</v>
       </c>
       <c r="C64" t="s">
-        <v>190</v>
+        <v>151</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>5</v>
-      </c>
-      <c r="B65" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C65" t="s">
-        <v>4</v>
+        <v>188</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>192</v>
+        <v>5</v>
       </c>
       <c r="B66" t="s">
-        <v>193</v>
+        <v>152</v>
       </c>
       <c r="C66" t="s">
-        <v>194</v>
+        <v>4</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>153</v>
+      </c>
+      <c r="B67" t="s">
+        <v>154</v>
+      </c>
+      <c r="C67" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>3</v>
       </c>
-      <c r="B67" t="s">
-        <v>195</v>
-      </c>
-      <c r="C67" t="s">
+      <c r="B68" t="s">
+        <v>156</v>
+      </c>
+      <c r="C68" t="s">
         <v>2</v>
       </c>
     </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>193</v>
+      </c>
+      <c r="C69" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>1</v>
+      </c>
+      <c r="B70" t="s">
+        <v>157</v>
+      </c>
+      <c r="C70" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:C68">
+  <sortState ref="A2:C71">
     <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Prepared Spreadsheet for Devlery
Updated the Topical Areas to match current 3.10 categories. Update the
END TIME to replicate the START TIME. Programmers can override with
longer or shorter end times, but Ical will populate some End time either
way.
</commit_message>
<xml_diff>
--- a/20140722_TOPICAL_AREAS_SHEET_REVISION.xlsx
+++ b/20140722_TOPICAL_AREAS_SHEET_REVISION.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="197">
   <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Writing:/user/agrp_calsuite-MainCampus/Writing</t>
   </si>
@@ -256,15 +256,6 @@
     <t>402881e6-20a21413-0120-a23d71e5-00000015</t>
   </si>
   <si>
-    <t>Business</t>
-  </si>
-  <si>
-    <t>2a3e9efe-334bc29f-0133-f14fa578-00001df6</t>
-  </si>
-  <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Business:/user/agrp_calsuite-MainCampus/Business</t>
-  </si>
-  <si>
     <t>ff808181-1fd7389e-011f-d7389f33-00000012</t>
   </si>
   <si>
@@ -475,15 +466,6 @@
     <t>402881e6-20a21413-0120-a23e31ea-00000016</t>
   </si>
   <si>
-    <t>Teen Crafts</t>
-  </si>
-  <si>
-    <t>2a3e9efe-334bc29f-0133-bc4fcd2f-0000762c</t>
-  </si>
-  <si>
-    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Teen Crafts:/user/agrp_calsuite-MainCampus/Teen Crafts</t>
-  </si>
-  <si>
     <t>2a3e9efe-334bc29f-0133-79d748a2-000036b0</t>
   </si>
   <si>
@@ -611,6 +593,18 @@
   </si>
   <si>
     <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=Artober:/user/agrp_calsuite-MainCampus/series/Artober</t>
+  </si>
+  <si>
+    <t>series/African American History Month</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/African American History Month:/user/agrp_calsuite-MainCampus/series/African American History Month</t>
+  </si>
+  <si>
+    <t>series/Studio NPL</t>
+  </si>
+  <si>
+    <t>X-BEDEWORK-ALIAS;X-BEDEWORK-PARAM-DISPLAYNAME=series/Studio NPL:/user/agrp_calsuite-MainCampus/series/Studio NPL</t>
   </si>
 </sst>
 </file>
@@ -969,8 +963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1003,13 +997,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B3" t="s">
         <v>78</v>
       </c>
       <c r="C3" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1025,408 +1019,405 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C5" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" t="s">
         <v>80</v>
       </c>
-      <c r="B6" t="s">
-        <v>81</v>
-      </c>
       <c r="C6" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>69</v>
+        <v>158</v>
       </c>
       <c r="B7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C7" t="s">
-        <v>68</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C8" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>166</v>
-      </c>
-      <c r="B9" t="s">
-        <v>85</v>
+        <v>162</v>
       </c>
       <c r="C9" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>168</v>
+        <v>67</v>
+      </c>
+      <c r="B10" t="s">
+        <v>83</v>
       </c>
       <c r="C10" t="s">
-        <v>169</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>67</v>
+        <v>164</v>
       </c>
       <c r="B11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C11" t="s">
-        <v>66</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>170</v>
-      </c>
-      <c r="B12" t="s">
-        <v>87</v>
+        <v>166</v>
       </c>
       <c r="C12" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>172</v>
+        <v>65</v>
+      </c>
+      <c r="B13" t="s">
+        <v>85</v>
       </c>
       <c r="C13" t="s">
-        <v>173</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>65</v>
-      </c>
-      <c r="B14" t="s">
-        <v>88</v>
+        <v>168</v>
       </c>
       <c r="C14" t="s">
-        <v>64</v>
+        <v>169</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>174</v>
+        <v>63</v>
+      </c>
+      <c r="B15" t="s">
+        <v>86</v>
       </c>
       <c r="C15" t="s">
-        <v>175</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B16" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B17" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B18" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C18" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B19" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B20" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C20" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B22" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C22" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B23" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C23" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B24" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B25" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C25" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B26" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C26" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B27" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B28" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C28" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>170</v>
       </c>
       <c r="B29" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C29" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>176</v>
+        <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C30" t="s">
-        <v>104</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C32" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B33" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C33" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B34" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C34" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B35" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C35" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B36" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C36" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>23</v>
+        <v>171</v>
       </c>
       <c r="B37" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C37" t="s">
-        <v>22</v>
+        <v>172</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>177</v>
+        <v>21</v>
       </c>
       <c r="B38" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C38" t="s">
-        <v>178</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>21</v>
+        <v>110</v>
       </c>
       <c r="B39" t="s">
+        <v>111</v>
+      </c>
+      <c r="C39" t="s">
         <v>112</v>
-      </c>
-      <c r="C39" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>113</v>
-      </c>
-      <c r="B40" t="s">
-        <v>114</v>
+        <v>173</v>
       </c>
       <c r="C40" t="s">
-        <v>115</v>
+        <v>174</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>179</v>
+        <v>115</v>
+      </c>
+      <c r="B41" t="s">
+        <v>116</v>
       </c>
       <c r="C41" t="s">
-        <v>180</v>
+        <v>117</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>118</v>
-      </c>
-      <c r="B42" t="s">
-        <v>119</v>
+        <v>193</v>
       </c>
       <c r="C42" t="s">
-        <v>120</v>
+        <v>194</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1434,18 +1425,18 @@
         <v>19</v>
       </c>
       <c r="B43" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C43" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="C44" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1453,10 +1444,10 @@
         <v>18</v>
       </c>
       <c r="B45" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C45" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1464,10 +1455,10 @@
         <v>17</v>
       </c>
       <c r="B46" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C46" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -1475,29 +1466,29 @@
         <v>16</v>
       </c>
       <c r="B47" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C47" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B48" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C48" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="C49" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1505,18 +1496,18 @@
         <v>15</v>
       </c>
       <c r="B50" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C50" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="C51" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1524,10 +1515,10 @@
         <v>14</v>
       </c>
       <c r="B52" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C52" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1535,10 +1526,10 @@
         <v>13</v>
       </c>
       <c r="B53" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C53" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -1546,10 +1537,10 @@
         <v>11</v>
       </c>
       <c r="B54" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C54" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -1557,10 +1548,10 @@
         <v>12</v>
       </c>
       <c r="B55" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C55" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -1568,10 +1559,10 @@
         <v>10</v>
       </c>
       <c r="B56" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C56" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1579,10 +1570,10 @@
         <v>9</v>
       </c>
       <c r="B57" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C57" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -1595,95 +1586,92 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>185</v>
-      </c>
-      <c r="B59" t="s">
-        <v>146</v>
+        <v>189</v>
       </c>
       <c r="C59" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>8</v>
+        <v>179</v>
       </c>
       <c r="B60" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C60" t="s">
-        <v>197</v>
+        <v>180</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>189</v>
+        <v>8</v>
+      </c>
+      <c r="B61" t="s">
+        <v>144</v>
       </c>
       <c r="C61" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>191</v>
-      </c>
-      <c r="B62" t="s">
-        <v>122</v>
+        <v>183</v>
       </c>
       <c r="C62" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>7</v>
+        <v>185</v>
       </c>
       <c r="B63" t="s">
-        <v>148</v>
+        <v>119</v>
       </c>
       <c r="C63" t="s">
-        <v>149</v>
+        <v>186</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B64" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C64" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>187</v>
+        <v>6</v>
+      </c>
+      <c r="B65" t="s">
+        <v>147</v>
       </c>
       <c r="C65" t="s">
-        <v>188</v>
+        <v>148</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>5</v>
-      </c>
-      <c r="B66" t="s">
-        <v>152</v>
+        <v>181</v>
       </c>
       <c r="C66" t="s">
-        <v>4</v>
+        <v>182</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>153</v>
+        <v>5</v>
       </c>
       <c r="B67" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C67" t="s">
-        <v>155</v>
+        <v>4</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -1691,7 +1679,7 @@
         <v>3</v>
       </c>
       <c r="B68" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C68" t="s">
         <v>2</v>
@@ -1699,10 +1687,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="C69" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -1710,7 +1698,7 @@
         <v>1</v>
       </c>
       <c r="B70" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C70" t="s">
         <v>0</v>

</xml_diff>